<commit_message>
Households have young, middle, elderly structure.
</commit_message>
<xml_diff>
--- a/data/processed/poland/DW/households_count.xlsx
+++ b/data/processed/poland/DW/households_count.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="raw" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="processed" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,12 +21,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t xml:space="preserve">nb_of_people_in_household</t>
   </si>
   <si>
     <t xml:space="preserve">nb_of_households</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nb_of_people in these households</t>
+  </si>
+  <si>
+    <t xml:space="preserve">proportionally nb of people in each headcount household</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nb of people given current population size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nb of households to lodge current population</t>
   </si>
 </sst>
 </file>
@@ -115,13 +128,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -141,10 +158,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -162,6 +179,18 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -170,6 +199,22 @@
       <c r="B2" s="0" t="n">
         <v>92713</v>
       </c>
+      <c r="C2" s="0" t="n">
+        <f aca="false">B2*A2</f>
+        <v>92713</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <f aca="false">C2/$C$9</f>
+        <v>0.14853924843591</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <f aca="false">D2*$D$9</f>
+        <v>95303.8215712192</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <f aca="false">ROUND(E2/A2,0)</f>
+        <v>95304</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -178,6 +223,22 @@
       <c r="B3" s="0" t="n">
         <v>81495</v>
       </c>
+      <c r="C3" s="0" t="n">
+        <f aca="false">B3*A3</f>
+        <v>162990</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <f aca="false">C3/$C$9</f>
+        <v>0.261132873519021</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <f aca="false">D3*$D$9</f>
+        <v>167544.679579919</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <f aca="false">ROUND(E3/A3,0)</f>
+        <v>83772</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -186,6 +247,22 @@
       <c r="B4" s="0" t="n">
         <v>51620</v>
       </c>
+      <c r="C4" s="0" t="n">
+        <f aca="false">B4*A4</f>
+        <v>154860</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <f aca="false">C4/$C$9</f>
+        <v>0.248107471582034</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <f aca="false">D4*$D$9</f>
+        <v>159187.490519334</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <f aca="false">ROUND(E4/A4,0)</f>
+        <v>53062</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -194,6 +271,22 @@
       <c r="B5" s="0" t="n">
         <v>31719</v>
       </c>
+      <c r="C5" s="0" t="n">
+        <f aca="false">B5*A5</f>
+        <v>126876</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <f aca="false">C5/$C$9</f>
+        <v>0.203273172959073</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <f aca="false">D5*$D$9</f>
+        <v>130421.490682752</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <f aca="false">ROUND(E5/A5,0)</f>
+        <v>32605</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -202,6 +295,22 @@
       <c r="B6" s="0" t="n">
         <v>8312</v>
       </c>
+      <c r="C6" s="0" t="n">
+        <f aca="false">B6*A6</f>
+        <v>41560</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <f aca="false">C6/$C$9</f>
+        <v>0.0665849575032243</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <f aca="false">D6*$D$9</f>
+        <v>42721.3748287712</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <f aca="false">ROUND(E6/A6,0)</f>
+        <v>8544</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -210,6 +319,22 @@
       <c r="B7" s="0" t="n">
         <v>4688</v>
       </c>
+      <c r="C7" s="0" t="n">
+        <f aca="false">B7*A7</f>
+        <v>28128</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <f aca="false">C7/$C$9</f>
+        <v>0.0450650068491505</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <f aca="false">D7*$D$9</f>
+        <v>28914.0238494629</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <f aca="false">ROUND(E7/A7,0)</f>
+        <v>4819</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -217,6 +342,43 @@
       </c>
       <c r="B8" s="0" t="n">
         <v>2434</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <f aca="false">B8*A8</f>
+        <v>17038</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <f aca="false">C8/$C$9</f>
+        <v>0.0272972691515865</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <f aca="false">D8*$D$9</f>
+        <v>17514.118968542</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <f aca="false">ROUND(E8/A8,0)</f>
+        <v>2502</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="n">
+        <f aca="false">SUM(B2:B8)</f>
+        <v>272981</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <f aca="false">SUM(C2:C8)</f>
+        <v>624165</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>641607</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <f aca="false">SUM(E2:E8)</f>
+        <v>641607</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <f aca="false">SUM(F2:F8)</f>
+        <v>280608</v>
       </c>
     </row>
   </sheetData>
@@ -228,4 +390,98 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="3" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>95304</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>83772</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>53062</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>32605</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>8544</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>4819</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>2502</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>